<commit_message>
Reemplazar archivo con áreas de tipos de infraestructura en cantones, cambiar a negro el color del límite cantonal y actualizar dirección del sitio principal del proyecto
</commit_message>
<xml_diff>
--- a/data/infraestructura-cantones.xlsx
+++ b/data/infraestructura-cantones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Atlas_2\matrices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UAC\2022\ATLAS_2\METRICAS_CIIUDAD_VERDE_2023\finales\finales_Juliana\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE45B2F6-4FBE-42FB-AB37-E8E8D2F364ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC4A934-F463-42FF-AAC7-B32E0030572F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{642B292C-E1AA-4A91-A22C-EAC34BB6DBE5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{642B292C-E1AA-4A91-A22C-EAC34BB6DBE5}"/>
   </bookViews>
   <sheets>
     <sheet name="cantones" sheetId="1" r:id="rId1"/>
@@ -599,32 +599,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E03E6D-C743-4E36-8287-F6BEDEFC5EB7}">
-  <dimension ref="A1:AN33"/>
+  <dimension ref="A1:AN34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" customWidth="1"/>
-    <col min="2" max="3" width="15.36328125" customWidth="1"/>
-    <col min="4" max="5" width="15.1796875" customWidth="1"/>
-    <col min="6" max="7" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.21875" customWidth="1"/>
+    <col min="6" max="7" width="19.44140625" customWidth="1"/>
     <col min="8" max="9" width="20" customWidth="1"/>
-    <col min="10" max="11" width="19.6328125" customWidth="1"/>
-    <col min="12" max="13" width="17.26953125" customWidth="1"/>
-    <col min="14" max="15" width="20.90625" customWidth="1"/>
-    <col min="16" max="17" width="20.1796875" customWidth="1"/>
-    <col min="18" max="19" width="15.08984375" customWidth="1"/>
-    <col min="28" max="29" width="15.54296875" customWidth="1"/>
-    <col min="30" max="31" width="14.08984375" customWidth="1"/>
-    <col min="32" max="33" width="12.6328125" customWidth="1"/>
-    <col min="38" max="39" width="14.54296875" customWidth="1"/>
-    <col min="40" max="40" width="13.7265625" customWidth="1"/>
+    <col min="10" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="13" width="17.21875" customWidth="1"/>
+    <col min="14" max="15" width="20.88671875" customWidth="1"/>
+    <col min="16" max="17" width="20.21875" customWidth="1"/>
+    <col min="18" max="19" width="15.109375" customWidth="1"/>
+    <col min="28" max="29" width="15.5546875" customWidth="1"/>
+    <col min="30" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="33" width="12.6640625" customWidth="1"/>
+    <col min="38" max="39" width="14.5546875" customWidth="1"/>
+    <col min="40" max="40" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -699,69 +699,69 @@
       <c r="AL1" s="4"/>
       <c r="AN1" s="4"/>
     </row>
-    <row r="2" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>3.8407680000000002</v>
+        <v>21.157056000000001</v>
       </c>
       <c r="C2" s="6">
-        <v>3.09456</v>
+        <v>15.427584</v>
       </c>
       <c r="D2" s="6">
-        <v>35.226288000000004</v>
+        <v>35.584992</v>
       </c>
       <c r="E2" s="6">
-        <v>25.098768</v>
+        <v>23.711760000000002</v>
       </c>
       <c r="F2" s="6">
-        <v>180.09316799999999</v>
+        <v>168.53025600000001</v>
       </c>
       <c r="G2" s="6">
-        <v>33.185088</v>
+        <v>32.922864000000004</v>
       </c>
       <c r="H2" s="6">
-        <v>425.54966399999995</v>
+        <v>418.99536000000001</v>
       </c>
       <c r="I2" s="6">
-        <v>500.84654400000005</v>
+        <v>505.048608</v>
       </c>
       <c r="J2" s="6">
-        <v>405.675072</v>
+        <v>386.11123199999997</v>
       </c>
       <c r="K2" s="6">
-        <v>289.35273599999999</v>
+        <v>266.66697599999998</v>
       </c>
       <c r="L2" s="6">
-        <v>0</v>
+        <v>26.049167999999998</v>
       </c>
       <c r="M2" s="6">
-        <v>7.339103999999999</v>
+        <v>7.3298880000000004</v>
       </c>
       <c r="N2" s="6">
-        <v>0</v>
+        <v>1.2960000000000001E-3</v>
       </c>
       <c r="O2" s="6">
-        <v>0.74059200000000003</v>
+        <v>0.73843199999999998</v>
       </c>
       <c r="P2" s="6">
-        <v>1206.3509279999998</v>
+        <v>1187.9416800000001</v>
       </c>
       <c r="Q2" s="6">
-        <v>1024.9724160000001</v>
+        <v>1020.0510720000001</v>
       </c>
       <c r="R2" s="6">
-        <v>167.26593600000001</v>
+        <v>163.47844799999999</v>
       </c>
       <c r="S2" s="6">
-        <v>84.292991999999998</v>
+        <v>94.021631999999997</v>
       </c>
       <c r="T2" s="6">
-        <v>20.42136</v>
+        <v>26.440128000000001</v>
       </c>
       <c r="U2" s="6">
-        <v>4.596336</v>
+        <v>17.738783999999999</v>
       </c>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -782,69 +782,69 @@
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
     </row>
-    <row r="3" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>0.61660800000000004</v>
+        <v>62.047727999999999</v>
       </c>
       <c r="C3" s="6">
-        <v>0</v>
+        <v>46.020240000000001</v>
       </c>
       <c r="D3" s="6">
-        <v>0</v>
+        <v>0.59673599999999993</v>
       </c>
       <c r="E3" s="6">
-        <v>91.495871999999991</v>
+        <v>86.454143999999999</v>
       </c>
       <c r="F3" s="6">
-        <v>184.24943999999999</v>
+        <v>171.919296</v>
       </c>
       <c r="G3" s="6">
-        <v>83.695104000000001</v>
+        <v>80.763120000000001</v>
       </c>
       <c r="H3" s="6">
-        <v>381.156048</v>
+        <v>378.89740799999998</v>
       </c>
       <c r="I3" s="6">
-        <v>772.55726399999992</v>
+        <v>773.002656</v>
       </c>
       <c r="J3" s="6">
-        <v>140.09601599999999</v>
+        <v>137.379456</v>
       </c>
       <c r="K3" s="6">
-        <v>361.04284799999999</v>
+        <v>343.99915199999998</v>
       </c>
       <c r="L3" s="6">
-        <v>6.4224000000000003E-2</v>
+        <v>28.830384000000002</v>
       </c>
       <c r="M3" s="6">
-        <v>40.296384000000003</v>
+        <v>35.308368000000002</v>
       </c>
       <c r="N3" s="6">
-        <v>0</v>
+        <v>1.0467360000000001</v>
       </c>
       <c r="O3" s="6">
-        <v>3.046176</v>
+        <v>2.9563200000000003</v>
       </c>
       <c r="P3" s="6">
-        <v>1963.3068000000001</v>
+        <v>1898.2817280000002</v>
       </c>
       <c r="Q3" s="6">
-        <v>1474.1688960000001</v>
+        <v>1427.6316960000001</v>
       </c>
       <c r="R3" s="6">
-        <v>496.28001599999999</v>
+        <v>485.37244800000002</v>
       </c>
       <c r="S3" s="6">
-        <v>134.07220800000002</v>
+        <v>138.58819199999999</v>
       </c>
       <c r="T3" s="6">
-        <v>5.2606080000000004</v>
+        <v>16.450559999999999</v>
       </c>
       <c r="U3" s="6">
-        <v>4.0836959999999998</v>
+        <v>20.092751999999997</v>
       </c>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
@@ -865,69 +865,69 @@
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
     </row>
-    <row r="4" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="6">
-        <v>0.622224</v>
+        <v>8.1080640000000006</v>
       </c>
       <c r="C4" s="6">
-        <v>0</v>
+        <v>11.458944000000001</v>
       </c>
       <c r="D4" s="6">
-        <v>0</v>
+        <v>4.104E-2</v>
       </c>
       <c r="E4" s="6">
-        <v>92.941199999999995</v>
+        <v>87.294240000000002</v>
       </c>
       <c r="F4" s="6">
-        <v>68.331744</v>
+        <v>65.052719999999994</v>
       </c>
       <c r="G4" s="6">
-        <v>162.08049599999998</v>
+        <v>160.17451200000002</v>
       </c>
       <c r="H4" s="6">
-        <v>145.12752</v>
+        <v>142.00847999999999</v>
       </c>
       <c r="I4" s="6">
-        <v>132.40310400000001</v>
+        <v>144.29275200000001</v>
       </c>
       <c r="J4" s="6">
-        <v>249.44673599999999</v>
+        <v>240.867504</v>
       </c>
       <c r="K4" s="6">
-        <v>367.445808</v>
+        <v>356.75078400000001</v>
       </c>
       <c r="L4" s="6">
-        <v>1.4057280000000001</v>
+        <v>14.667407999999998</v>
       </c>
       <c r="M4" s="6">
-        <v>67.637231999999997</v>
+        <v>64.590768000000011</v>
       </c>
       <c r="N4" s="6">
-        <v>10.995984</v>
+        <v>11.941488</v>
       </c>
       <c r="O4" s="6">
-        <v>0.82022399999999995</v>
+        <v>0.81835200000000008</v>
       </c>
       <c r="P4" s="6">
-        <v>471.76300800000001</v>
+        <v>464.17694400000005</v>
       </c>
       <c r="Q4" s="6">
-        <v>483.83769599999999</v>
+        <v>477.45907199999999</v>
       </c>
       <c r="R4" s="6">
-        <v>387.898416</v>
+        <v>385.42953599999998</v>
       </c>
       <c r="S4" s="6">
-        <v>7.8494399999999995</v>
+        <v>12.196512</v>
       </c>
       <c r="T4" s="6">
-        <v>0.68515200000000009</v>
+        <v>1.6634880000000001</v>
       </c>
       <c r="U4" s="6">
-        <v>3.7451519999999996</v>
+        <v>6.0130080000000001</v>
       </c>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
@@ -948,69 +948,69 @@
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
     </row>
-    <row r="5" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6">
-        <v>0</v>
+        <v>14.202576000000001</v>
       </c>
       <c r="C5" s="6">
-        <v>0</v>
+        <v>11.97</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>0.124128</v>
       </c>
       <c r="E5" s="6">
-        <v>15.923807999999999</v>
+        <v>15.495551999999998</v>
       </c>
       <c r="F5" s="6">
-        <v>60.795792000000006</v>
+        <v>57.604752000000005</v>
       </c>
       <c r="G5" s="6">
-        <v>64.233648000000002</v>
+        <v>63.106128000000005</v>
       </c>
       <c r="H5" s="6">
-        <v>146.97316799999999</v>
+        <v>143.766864</v>
       </c>
       <c r="I5" s="6">
-        <v>140.18299199999998</v>
+        <v>140.64796799999999</v>
       </c>
       <c r="J5" s="6">
-        <v>134.02425600000001</v>
+        <v>133.16198400000002</v>
       </c>
       <c r="K5" s="6">
-        <v>313.78032000000002</v>
+        <v>306.74505600000003</v>
       </c>
       <c r="L5" s="6">
-        <v>0.61055999999999999</v>
+        <v>9.4933440000000004</v>
       </c>
       <c r="M5" s="6">
-        <v>2.2000319999999998</v>
+        <v>1.504656</v>
       </c>
       <c r="N5" s="6">
-        <v>0</v>
+        <v>0.249696</v>
       </c>
       <c r="O5" s="6">
-        <v>0.11707200000000001</v>
+        <v>0.116496</v>
       </c>
       <c r="P5" s="6">
-        <v>829.27008000000001</v>
+        <v>814.86504000000002</v>
       </c>
       <c r="Q5" s="6">
-        <v>909.54662400000007</v>
+        <v>898.07414399999993</v>
       </c>
       <c r="R5" s="6">
-        <v>307.67817599999995</v>
+        <v>305.798112</v>
       </c>
       <c r="S5" s="6">
-        <v>30.751776</v>
+        <v>33.753168000000002</v>
       </c>
       <c r="T5" s="6">
-        <v>1.9408319999999999</v>
+        <v>4.7181600000000001</v>
       </c>
       <c r="U5" s="6">
-        <v>2.3767200000000002</v>
+        <v>5.3108639999999996</v>
       </c>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
@@ -1031,69 +1031,69 @@
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
-    <row r="6" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6">
-        <v>0</v>
+        <v>18.014832000000002</v>
       </c>
       <c r="C6" s="6">
-        <v>0</v>
+        <v>12.383424</v>
       </c>
       <c r="D6" s="6">
-        <v>0</v>
+        <v>0.16358399999999998</v>
       </c>
       <c r="E6" s="6">
-        <v>22.256640000000001</v>
+        <v>21.411792000000002</v>
       </c>
       <c r="F6" s="6">
-        <v>95.658192</v>
+        <v>88.201152000000008</v>
       </c>
       <c r="G6" s="6">
-        <v>20.707056000000001</v>
+        <v>20.370671999999999</v>
       </c>
       <c r="H6" s="6">
-        <v>293.99759999999998</v>
+        <v>289.33430400000003</v>
       </c>
       <c r="I6" s="6">
-        <v>245.49724799999998</v>
+        <v>247.02364800000001</v>
       </c>
       <c r="J6" s="6">
-        <v>75.438000000000002</v>
+        <v>69.138431999999995</v>
       </c>
       <c r="K6" s="6">
-        <v>342.00950399999999</v>
+        <v>330.70867200000004</v>
       </c>
       <c r="L6" s="6">
-        <v>0</v>
+        <v>13.186368</v>
       </c>
       <c r="M6" s="6">
-        <v>25.337951999999998</v>
+        <v>22.592304000000002</v>
       </c>
       <c r="N6" s="6">
-        <v>4.236192</v>
+        <v>3.9993120000000002</v>
       </c>
       <c r="O6" s="6">
-        <v>1.7212319999999999</v>
+        <v>0.84945599999999999</v>
       </c>
       <c r="P6" s="6">
-        <v>896.44996800000001</v>
+        <v>878.09558400000003</v>
       </c>
       <c r="Q6" s="6">
-        <v>598.29652800000008</v>
+        <v>590.67115200000001</v>
       </c>
       <c r="R6" s="6">
-        <v>185.075424</v>
+        <v>181.46865600000001</v>
       </c>
       <c r="S6" s="6">
-        <v>48.620591999999995</v>
+        <v>59.375376000000003</v>
       </c>
       <c r="T6" s="6">
-        <v>7.3520640000000004</v>
+        <v>10.147536000000001</v>
       </c>
       <c r="U6" s="6">
-        <v>5.4378720000000005</v>
+        <v>10.978128</v>
       </c>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
@@ -1114,69 +1114,69 @@
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6">
-        <v>0</v>
+        <v>2.4354720000000003</v>
       </c>
       <c r="C7" s="6">
-        <v>0</v>
+        <v>0.84499199999999997</v>
       </c>
       <c r="D7" s="6">
-        <v>72.61099200000001</v>
+        <v>72.30528000000001</v>
       </c>
       <c r="E7" s="6">
-        <v>75.264911999999995</v>
+        <v>74.871791999999999</v>
       </c>
       <c r="F7" s="6">
-        <v>147.008736</v>
+        <v>142.94448</v>
       </c>
       <c r="G7" s="6">
-        <v>356.091408</v>
+        <v>354.90225600000002</v>
       </c>
       <c r="H7" s="6">
-        <v>219.69820799999999</v>
+        <v>217.86192000000003</v>
       </c>
       <c r="I7" s="6">
-        <v>166.21617599999999</v>
+        <v>174.27196799999999</v>
       </c>
       <c r="J7" s="6">
         <v>0</v>
       </c>
       <c r="K7" s="6">
-        <v>3000.5507520000001</v>
+        <v>2710.5668639999999</v>
       </c>
       <c r="L7" s="6">
-        <v>12.706847999999999</v>
+        <v>305.04758399999997</v>
       </c>
       <c r="M7" s="6">
-        <v>1023.1080480000001</v>
+        <v>1017.8818560000001</v>
       </c>
       <c r="N7" s="6">
-        <v>29.465423999999999</v>
+        <v>29.856096000000001</v>
       </c>
       <c r="O7" s="6">
-        <v>5.5216799999999999</v>
+        <v>5.4904320000000002</v>
       </c>
       <c r="P7" s="6">
-        <v>614.88892800000008</v>
+        <v>613.56355199999996</v>
       </c>
       <c r="Q7" s="6">
-        <v>790.31433600000003</v>
+        <v>789.48144000000002</v>
       </c>
       <c r="R7" s="6">
-        <v>484.14916799999997</v>
+        <v>479.91729600000002</v>
       </c>
       <c r="S7" s="6">
-        <v>64.171440000000004</v>
+        <v>67.522751999999997</v>
       </c>
       <c r="T7" s="6">
-        <v>0.85276800000000008</v>
+        <v>0.93873600000000001</v>
       </c>
       <c r="U7" s="6">
-        <v>3.8504160000000005</v>
+        <v>5.7788639999999996</v>
       </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -1197,69 +1197,69 @@
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6">
-        <v>0</v>
+        <v>36.032544000000001</v>
       </c>
       <c r="C8" s="6">
-        <v>0</v>
+        <v>18.642960000000002</v>
       </c>
       <c r="D8" s="6">
-        <v>0</v>
+        <v>0.19353599999999999</v>
       </c>
       <c r="E8" s="6">
-        <v>41.255856000000001</v>
+        <v>40.652784000000004</v>
       </c>
       <c r="F8" s="6">
-        <v>69.810479999999998</v>
+        <v>65.317968000000008</v>
       </c>
       <c r="G8" s="6">
-        <v>14.176368</v>
+        <v>13.879007999999999</v>
       </c>
       <c r="H8" s="6">
-        <v>217.09108799999998</v>
+        <v>212.68152000000001</v>
       </c>
       <c r="I8" s="6">
-        <v>219.24993599999999</v>
+        <v>219.90182400000003</v>
       </c>
       <c r="J8" s="6">
-        <v>57.891599999999997</v>
+        <v>56.389247999999995</v>
       </c>
       <c r="K8" s="6">
-        <v>68.672592000000009</v>
+        <v>27.332496000000003</v>
       </c>
       <c r="L8" s="6">
-        <v>0</v>
+        <v>43.596144000000002</v>
       </c>
       <c r="M8" s="6">
-        <v>8.7547679999999986</v>
+        <v>8.57376</v>
       </c>
       <c r="N8" s="6">
-        <v>0</v>
+        <v>0.115344</v>
       </c>
       <c r="O8" s="6">
         <v>0</v>
       </c>
       <c r="P8" s="6">
-        <v>698.56459199999995</v>
+        <v>662.06505599999991</v>
       </c>
       <c r="Q8" s="6">
-        <v>472.61952000000002</v>
+        <v>454.19457599999998</v>
       </c>
       <c r="R8" s="6">
-        <v>233.90928</v>
+        <v>230.96102400000001</v>
       </c>
       <c r="S8" s="6">
-        <v>34.423056000000003</v>
+        <v>41.133167999999998</v>
       </c>
       <c r="T8" s="6">
-        <v>7.1013600000000006</v>
+        <v>8.2972800000000007</v>
       </c>
       <c r="U8" s="6">
-        <v>2.2341599999999997</v>
+        <v>5.8285439999999999</v>
       </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -1280,69 +1280,69 @@
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="6">
-        <v>0</v>
+        <v>1.7354880000000001</v>
       </c>
       <c r="C9" s="6">
-        <v>0</v>
+        <v>0.74231999999999998</v>
       </c>
       <c r="D9" s="6">
-        <v>15.922224</v>
+        <v>15.918768</v>
       </c>
       <c r="E9" s="6">
-        <v>112.26686399999998</v>
+        <v>111.94041599999998</v>
       </c>
       <c r="F9" s="6">
-        <v>94.407696000000001</v>
+        <v>93.664224000000004</v>
       </c>
       <c r="G9" s="6">
-        <v>296.83699200000001</v>
+        <v>296.91518400000001</v>
       </c>
       <c r="H9" s="6">
-        <v>103.493808</v>
+        <v>103.369392</v>
       </c>
       <c r="I9" s="6">
-        <v>44.780112000000003</v>
+        <v>47.113632000000003</v>
       </c>
       <c r="J9" s="6">
         <v>0.9037440000000001</v>
       </c>
       <c r="K9" s="6">
-        <v>3764.5260479999997</v>
+        <v>3686.9074560000004</v>
       </c>
       <c r="L9" s="6">
-        <v>0</v>
+        <v>75.034656000000012</v>
       </c>
       <c r="M9" s="6">
-        <v>1141.6619519999999</v>
+        <v>1149.036912</v>
       </c>
       <c r="N9" s="6">
-        <v>7.1999999999999998E-3</v>
+        <v>5.1552000000000001E-2</v>
       </c>
       <c r="O9" s="6">
-        <v>4.5465119999999999</v>
+        <v>4.5476640000000002</v>
       </c>
       <c r="P9" s="6">
-        <v>933.36984000000007</v>
+        <v>931.77331199999992</v>
       </c>
       <c r="Q9" s="6">
-        <v>845.72654399999999</v>
+        <v>844.92071999999996</v>
       </c>
       <c r="R9" s="6">
-        <v>478.41422400000005</v>
+        <v>471.45585599999998</v>
       </c>
       <c r="S9" s="6">
-        <v>7.1000639999999997</v>
+        <v>7.4538720000000005</v>
       </c>
       <c r="T9" s="6">
-        <v>0.387936</v>
+        <v>0.39571200000000001</v>
       </c>
       <c r="U9" s="6">
-        <v>2.357856</v>
+        <v>2.8997280000000001</v>
       </c>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -1363,69 +1363,69 @@
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
     </row>
-    <row r="10" spans="1:40" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="6">
-        <v>0</v>
+        <v>15.692688</v>
       </c>
       <c r="C10" s="6">
-        <v>0</v>
+        <v>8.5098240000000001</v>
       </c>
       <c r="D10" s="6">
-        <v>0</v>
+        <v>0.22896</v>
       </c>
       <c r="E10" s="6">
-        <v>73.870559999999998</v>
+        <v>72.780480000000011</v>
       </c>
       <c r="F10" s="6">
-        <v>106.73136000000001</v>
+        <v>100.820592</v>
       </c>
       <c r="G10" s="6">
-        <v>37.013040000000004</v>
+        <v>36.734687999999998</v>
       </c>
       <c r="H10" s="6">
-        <v>272.33769599999999</v>
+        <v>267.12576000000001</v>
       </c>
       <c r="I10" s="6">
-        <v>231.1848</v>
+        <v>229.69943999999998</v>
       </c>
       <c r="J10" s="6">
-        <v>13.614192000000001</v>
+        <v>12.311135999999999</v>
       </c>
       <c r="K10" s="6">
-        <v>1365.736752</v>
+        <v>1362.078</v>
       </c>
       <c r="L10" s="6">
-        <v>1.1748959999999999</v>
+        <v>13.023216</v>
       </c>
       <c r="M10" s="6">
-        <v>3.7303199999999999</v>
+        <v>3.6858239999999998</v>
       </c>
       <c r="N10" s="6">
-        <v>0.32097600000000004</v>
+        <v>0.34531200000000001</v>
       </c>
       <c r="O10" s="6">
-        <v>0.45446400000000003</v>
+        <v>0.45374399999999998</v>
       </c>
       <c r="P10" s="6">
-        <v>1083.1790880000001</v>
+        <v>1066.2330240000001</v>
       </c>
       <c r="Q10" s="6">
-        <v>1429.0195679999999</v>
+        <v>1419.7246560000001</v>
       </c>
       <c r="R10" s="6">
-        <v>514.249776</v>
+        <v>506.27059199999997</v>
       </c>
       <c r="S10" s="6">
-        <v>45.423648</v>
+        <v>56.843280000000007</v>
       </c>
       <c r="T10" s="6">
-        <v>7.0030080000000003</v>
+        <v>8.0952479999999998</v>
       </c>
       <c r="U10" s="6">
-        <v>2.8271519999999999</v>
+        <v>7.1724960000000006</v>
       </c>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
@@ -1446,69 +1446,69 @@
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
     </row>
-    <row r="11" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="6">
-        <v>0.216144</v>
+        <v>5.1173279999999997</v>
       </c>
       <c r="C11" s="6">
-        <v>0.96796800000000005</v>
+        <v>2.98584</v>
       </c>
       <c r="D11" s="6">
-        <v>0</v>
+        <v>0.18835199999999999</v>
       </c>
       <c r="E11" s="6">
-        <v>27.970128000000003</v>
+        <v>26.649359999999998</v>
       </c>
       <c r="F11" s="6">
-        <v>65.530656000000008</v>
+        <v>62.434656000000004</v>
       </c>
       <c r="G11" s="6">
-        <v>35.57808</v>
+        <v>34.419024</v>
       </c>
       <c r="H11" s="6">
-        <v>214.018992</v>
+        <v>212.11502400000003</v>
       </c>
       <c r="I11" s="6">
-        <v>409.25059199999998</v>
+        <v>415.99367999999998</v>
       </c>
       <c r="J11" s="6">
-        <v>18.484127999999998</v>
+        <v>17.843039999999998</v>
       </c>
       <c r="K11" s="6">
-        <v>97.298352000000008</v>
+        <v>96.745968000000005</v>
       </c>
       <c r="L11" s="6">
-        <v>2.357856</v>
+        <v>4.3444799999999999</v>
       </c>
       <c r="M11" s="6">
-        <v>26.720208000000003</v>
+        <v>18.017712</v>
       </c>
       <c r="N11" s="6">
-        <v>0</v>
+        <v>0.22593600000000003</v>
       </c>
       <c r="O11" s="6">
-        <v>0.76636800000000005</v>
+        <v>0.59472000000000003</v>
       </c>
       <c r="P11" s="6">
-        <v>98.804736000000005</v>
+        <v>93.337343999999987</v>
       </c>
       <c r="Q11" s="6">
-        <v>122.54875200000001</v>
+        <v>120.568032</v>
       </c>
       <c r="R11" s="6">
-        <v>73.222992000000005</v>
+        <v>70.698527999999996</v>
       </c>
       <c r="S11" s="6">
-        <v>34.157375999999999</v>
+        <v>40.932575999999997</v>
       </c>
       <c r="T11" s="6">
-        <v>7.1506080000000001</v>
+        <v>7.6191839999999997</v>
       </c>
       <c r="U11" s="6">
-        <v>3.2241599999999999</v>
+        <v>7.4375999999999998</v>
       </c>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -1529,69 +1529,69 @@
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
     </row>
-    <row r="12" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="6">
-        <v>0</v>
+        <v>24.818832</v>
       </c>
       <c r="C12" s="6">
-        <v>0</v>
+        <v>10.937519999999999</v>
       </c>
       <c r="D12" s="6">
-        <v>0</v>
+        <v>9.1151999999999997E-2</v>
       </c>
       <c r="E12" s="6">
-        <v>35.040384000000003</v>
+        <v>33.809328000000001</v>
       </c>
       <c r="F12" s="6">
-        <v>71.996976000000004</v>
+        <v>69.559343999999996</v>
       </c>
       <c r="G12" s="6">
-        <v>106.46784</v>
+        <v>105.08543999999999</v>
       </c>
       <c r="H12" s="6">
-        <v>101.085408</v>
+        <v>100.28217600000001</v>
       </c>
       <c r="I12" s="6">
-        <v>161.04715200000001</v>
+        <v>161.761392</v>
       </c>
       <c r="J12" s="6">
-        <v>11.053728</v>
+        <v>11.045664</v>
       </c>
       <c r="K12" s="6">
-        <v>860.85</v>
+        <v>708.32851200000005</v>
       </c>
       <c r="L12" s="6">
-        <v>0</v>
+        <v>19.747007999999997</v>
       </c>
       <c r="M12" s="6">
-        <v>5.1870240000000001</v>
+        <v>4.8764160000000007</v>
       </c>
       <c r="N12" s="6">
-        <v>0</v>
+        <v>3.7727999999999998E-2</v>
       </c>
       <c r="O12" s="6">
-        <v>1.0270079999999999</v>
+        <v>1.0247040000000001</v>
       </c>
       <c r="P12" s="6">
-        <v>2419.986672</v>
+        <v>2393.0141760000001</v>
       </c>
       <c r="Q12" s="6">
-        <v>1849.251888</v>
+        <v>1837.5033600000002</v>
       </c>
       <c r="R12" s="6">
-        <v>715.92465599999991</v>
+        <v>851.02228800000012</v>
       </c>
       <c r="S12" s="6">
-        <v>42.107040000000005</v>
+        <v>45.230831999999999</v>
       </c>
       <c r="T12" s="6">
-        <v>1.242864</v>
+        <v>2.0125439999999997</v>
       </c>
       <c r="U12" s="6">
-        <v>2.7097919999999998</v>
+        <v>5.6453760000000006</v>
       </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -1612,42 +1612,42 @@
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
     </row>
-    <row r="13" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="6">
-        <v>3.3153120000000005</v>
+        <v>10.769183999999999</v>
       </c>
       <c r="C13" s="6">
-        <v>3.3238080000000001</v>
+        <v>7.6726080000000003</v>
       </c>
       <c r="D13" s="6">
-        <v>0</v>
+        <v>0.81431999999999993</v>
       </c>
       <c r="E13" s="6">
-        <v>6.5846880000000008</v>
+        <v>6.1153919999999999</v>
       </c>
       <c r="F13" s="6">
-        <v>125.425296</v>
+        <v>116.572896</v>
       </c>
       <c r="G13" s="6">
-        <v>19.908287999999999</v>
+        <v>19.098288</v>
       </c>
       <c r="H13" s="6">
-        <v>386.51140800000002</v>
+        <v>382.36276800000002</v>
       </c>
       <c r="I13" s="6">
-        <v>423.39009599999997</v>
+        <v>421.96910400000002</v>
       </c>
       <c r="J13" s="6">
-        <v>90.081360000000004</v>
+        <v>87.282719999999998</v>
       </c>
       <c r="K13" s="6">
-        <v>13.652064000000001</v>
+        <v>12.067632000000001</v>
       </c>
       <c r="L13" s="6">
-        <v>0</v>
+        <v>2.5604640000000001</v>
       </c>
       <c r="M13" s="6">
         <v>0</v>
@@ -1656,25 +1656,25 @@
         <v>0</v>
       </c>
       <c r="O13" s="6">
-        <v>0.26913599999999999</v>
+        <v>0.26855999999999997</v>
       </c>
       <c r="P13" s="6">
-        <v>139.27032</v>
+        <v>131.92804799999999</v>
       </c>
       <c r="Q13" s="6">
-        <v>188.83166399999999</v>
+        <v>186.92884799999999</v>
       </c>
       <c r="R13" s="6">
-        <v>126.57974399999999</v>
+        <v>123.96182399999999</v>
       </c>
       <c r="S13" s="6">
-        <v>56.350368000000003</v>
+        <v>65.689775999999995</v>
       </c>
       <c r="T13" s="6">
-        <v>18.116783999999999</v>
+        <v>19.436831999999999</v>
       </c>
       <c r="U13" s="6">
-        <v>4.6465920000000001</v>
+        <v>10.761264000000001</v>
       </c>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -1695,69 +1695,69 @@
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
     </row>
-    <row r="14" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="6">
-        <v>0</v>
+        <v>16.072848</v>
       </c>
       <c r="C14" s="6">
-        <v>0</v>
+        <v>13.036175999999999</v>
       </c>
       <c r="D14" s="6">
-        <v>2.1067200000000001</v>
+        <v>2.20248</v>
       </c>
       <c r="E14" s="6">
-        <v>58.990464000000003</v>
+        <v>58.447295999999994</v>
       </c>
       <c r="F14" s="6">
-        <v>116.915328</v>
+        <v>112.73529599999999</v>
       </c>
       <c r="G14" s="6">
-        <v>220.91788799999998</v>
+        <v>219.03249600000001</v>
       </c>
       <c r="H14" s="6">
-        <v>230.78563199999999</v>
+        <v>229.49265600000001</v>
       </c>
       <c r="I14" s="6">
-        <v>244.536192</v>
+        <v>255.98851200000001</v>
       </c>
       <c r="J14" s="6">
-        <v>242.34321600000001</v>
+        <v>233.29627200000002</v>
       </c>
       <c r="K14" s="6">
-        <v>2282.6250719999998</v>
+        <v>2264.984496</v>
       </c>
       <c r="L14" s="6">
-        <v>2.4554879999999999</v>
+        <v>22.793039999999998</v>
       </c>
       <c r="M14" s="6">
-        <v>122.54428799999999</v>
+        <v>119.623392</v>
       </c>
       <c r="N14" s="6">
-        <v>13.696128</v>
+        <v>13.689360000000001</v>
       </c>
       <c r="O14" s="6">
-        <v>2.1513599999999999</v>
+        <v>2.1484799999999997</v>
       </c>
       <c r="P14" s="6">
-        <v>2141.2978559999997</v>
+        <v>2125.9702079999997</v>
       </c>
       <c r="Q14" s="6">
-        <v>1756.3429440000002</v>
+        <v>1745.5633920000002</v>
       </c>
       <c r="R14" s="6">
-        <v>825.59231999999997</v>
+        <v>822.54758400000003</v>
       </c>
       <c r="S14" s="6">
-        <v>84.704976000000002</v>
+        <v>88.033104000000009</v>
       </c>
       <c r="T14" s="6">
-        <v>2.4816959999999999</v>
+        <v>2.2955040000000002</v>
       </c>
       <c r="U14" s="6">
-        <v>5.857488</v>
+        <v>8.9552160000000001</v>
       </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
@@ -1778,69 +1778,69 @@
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
     </row>
-    <row r="15" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="6">
-        <v>0</v>
+        <v>40.818959999999997</v>
       </c>
       <c r="C15" s="6">
-        <v>0</v>
+        <v>89.128368000000009</v>
       </c>
       <c r="D15" s="6">
-        <v>0</v>
+        <v>0.12196800000000001</v>
       </c>
       <c r="E15" s="6">
-        <v>79.496783999999991</v>
+        <v>76.572288</v>
       </c>
       <c r="F15" s="6">
-        <v>109.30463999999999</v>
+        <v>105.33398400000002</v>
       </c>
       <c r="G15" s="6">
-        <v>305.59852799999999</v>
+        <v>303.002928</v>
       </c>
       <c r="H15" s="6">
-        <v>193.10688000000002</v>
+        <v>191.783232</v>
       </c>
       <c r="I15" s="6">
-        <v>331.96752000000004</v>
+        <v>531.77529600000003</v>
       </c>
       <c r="J15" s="6">
-        <v>1369.607904</v>
+        <v>1178.3187359999999</v>
       </c>
       <c r="K15" s="6">
-        <v>481.96857599999998</v>
+        <v>468.61588799999998</v>
       </c>
       <c r="L15" s="6">
-        <v>71.752319999999997</v>
+        <v>87.761088000000001</v>
       </c>
       <c r="M15" s="6">
-        <v>521.65987199999995</v>
+        <v>501.15686399999998</v>
       </c>
       <c r="N15" s="6">
-        <v>155.89368000000002</v>
+        <v>156.61080000000001</v>
       </c>
       <c r="O15" s="6">
-        <v>4.3682400000000001</v>
+        <v>4.9703040000000005</v>
       </c>
       <c r="P15" s="6">
-        <v>1187.215776</v>
+        <v>1144.9223999999999</v>
       </c>
       <c r="Q15" s="6">
-        <v>1097.3154240000001</v>
+        <v>1017.7341119999999</v>
       </c>
       <c r="R15" s="6">
-        <v>713.89800000000002</v>
+        <v>706.75632000000007</v>
       </c>
       <c r="S15" s="6">
-        <v>21.494016000000002</v>
+        <v>26.895167999999998</v>
       </c>
       <c r="T15" s="6">
-        <v>1.749312</v>
+        <v>3.1016159999999999</v>
       </c>
       <c r="U15" s="6">
-        <v>3.1134240000000002</v>
+        <v>14.188464000000002</v>
       </c>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
@@ -1861,69 +1861,69 @@
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
     </row>
-    <row r="16" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="6">
-        <v>0</v>
+        <v>4.3657919999999999</v>
       </c>
       <c r="C16" s="6">
-        <v>1.412496</v>
+        <v>15.094944</v>
       </c>
       <c r="D16" s="6">
-        <v>0</v>
+        <v>0.40968000000000004</v>
       </c>
       <c r="E16" s="6">
-        <v>3.7005120000000002</v>
+        <v>3.0419999999999998</v>
       </c>
       <c r="F16" s="6">
-        <v>54.295487999999999</v>
+        <v>47.749103999999996</v>
       </c>
       <c r="G16" s="6">
-        <v>33.777647999999999</v>
+        <v>40.173120000000004</v>
       </c>
       <c r="H16" s="6">
-        <v>162.29563200000001</v>
+        <v>156.61223999999999</v>
       </c>
       <c r="I16" s="6">
-        <v>182.31753600000002</v>
+        <v>186.19286399999999</v>
       </c>
       <c r="J16" s="6">
-        <v>146.806128</v>
+        <v>140.06001599999999</v>
       </c>
       <c r="K16" s="6">
-        <v>19.032335999999997</v>
+        <v>13.32216</v>
       </c>
       <c r="L16" s="6">
-        <v>0</v>
+        <v>6.1695359999999999</v>
       </c>
       <c r="M16" s="6">
-        <v>24.423264</v>
+        <v>22.235904000000001</v>
       </c>
       <c r="N16" s="6">
-        <v>1.0512000000000001E-2</v>
+        <v>1.057104</v>
       </c>
       <c r="O16" s="6">
         <v>0</v>
       </c>
       <c r="P16" s="6">
-        <v>14.721407999999998</v>
+        <v>10.329408000000001</v>
       </c>
       <c r="Q16" s="6">
-        <v>54.464543999999997</v>
+        <v>42.259679999999996</v>
       </c>
       <c r="R16" s="6">
-        <v>106.870176</v>
+        <v>100.769904</v>
       </c>
       <c r="S16" s="6">
-        <v>15.848495999999999</v>
+        <v>23.971679999999999</v>
       </c>
       <c r="T16" s="6">
-        <v>11.708784</v>
+        <v>13.229135999999999</v>
       </c>
       <c r="U16" s="6">
-        <v>2.1329279999999997</v>
+        <v>6.8205600000000004</v>
       </c>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -1944,69 +1944,69 @@
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
     </row>
-    <row r="17" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="6">
-        <v>0</v>
+        <v>323.95881600000001</v>
       </c>
       <c r="C17" s="6">
-        <v>0</v>
+        <v>11.378736</v>
       </c>
       <c r="D17" s="6">
-        <v>32.038848000000002</v>
+        <v>32.193071999999994</v>
       </c>
       <c r="E17" s="6">
-        <v>146.08439999999999</v>
+        <v>144.38808</v>
       </c>
       <c r="F17" s="6">
-        <v>199.42358400000001</v>
+        <v>192.93753600000002</v>
       </c>
       <c r="G17" s="6">
-        <v>441.02505599999995</v>
+        <v>438.67079999999999</v>
       </c>
       <c r="H17" s="6">
-        <v>318.31804799999998</v>
+        <v>317.25230399999998</v>
       </c>
       <c r="I17" s="6">
-        <v>211.75963199999998</v>
+        <v>219.01795200000001</v>
       </c>
       <c r="J17" s="6">
-        <v>508.87454400000001</v>
+        <v>506.24135999999999</v>
       </c>
       <c r="K17" s="6">
-        <v>3434.3981280000003</v>
+        <v>3419.3456639999999</v>
       </c>
       <c r="L17" s="6">
-        <v>8.0497440000000005</v>
+        <v>24.236784</v>
       </c>
       <c r="M17" s="6">
-        <v>847.11398399999996</v>
+        <v>867.01780800000006</v>
       </c>
       <c r="N17" s="6">
-        <v>151.11403200000001</v>
+        <v>151.66800000000001</v>
       </c>
       <c r="O17" s="6">
-        <v>294.42513600000001</v>
+        <v>294.22368</v>
       </c>
       <c r="P17" s="6">
-        <v>5261.9293440000001</v>
+        <v>4934.5175520000003</v>
       </c>
       <c r="Q17" s="6">
-        <v>3347.9441280000001</v>
+        <v>3335.7522239999998</v>
       </c>
       <c r="R17" s="6">
-        <v>1508.682384</v>
+        <v>1492.6564800000001</v>
       </c>
       <c r="S17" s="6">
-        <v>63.147024000000002</v>
+        <v>67.096800000000002</v>
       </c>
       <c r="T17" s="6">
-        <v>7.572960000000001</v>
+        <v>7.5456000000000003</v>
       </c>
       <c r="U17" s="6">
-        <v>8.0804159999999996</v>
+        <v>10.406303999999999</v>
       </c>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -2027,69 +2027,69 @@
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
     </row>
-    <row r="18" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6">
-        <v>0.142128</v>
+        <v>9.2711520000000007</v>
       </c>
       <c r="C18" s="6">
-        <v>0.140544</v>
+        <v>4.4395199999999999</v>
       </c>
       <c r="D18" s="6">
-        <v>0</v>
+        <v>0.22017600000000001</v>
       </c>
       <c r="E18" s="6">
-        <v>29.127455999999999</v>
+        <v>28.428191999999999</v>
       </c>
       <c r="F18" s="6">
-        <v>160.18315200000001</v>
+        <v>151.08494400000001</v>
       </c>
       <c r="G18" s="6">
-        <v>22.160736</v>
+        <v>21.413376</v>
       </c>
       <c r="H18" s="6">
-        <v>454.71715199999994</v>
+        <v>448.24478399999998</v>
       </c>
       <c r="I18" s="6">
-        <v>409.975056</v>
+        <v>415.99367999999998</v>
       </c>
       <c r="J18" s="6">
-        <v>38.009376000000003</v>
+        <v>30.361968000000001</v>
       </c>
       <c r="K18" s="6">
-        <v>440.33889599999998</v>
+        <v>436.50388799999996</v>
       </c>
       <c r="L18" s="6">
-        <v>0</v>
+        <v>6.4994399999999999</v>
       </c>
       <c r="M18" s="6">
-        <v>12.431232000000001</v>
+        <v>12.305375999999999</v>
       </c>
       <c r="N18" s="6">
-        <v>0</v>
+        <v>4.1327999999999997E-2</v>
       </c>
       <c r="O18" s="6">
         <v>0.19872000000000001</v>
       </c>
       <c r="P18" s="6">
-        <v>597.2364</v>
+        <v>587.43244800000002</v>
       </c>
       <c r="Q18" s="6">
-        <v>699.84417599999995</v>
+        <v>695.91758400000003</v>
       </c>
       <c r="R18" s="6">
-        <v>189.76953600000002</v>
+        <v>186.09753600000002</v>
       </c>
       <c r="S18" s="6">
-        <v>59.64264</v>
+        <v>71.762831999999989</v>
       </c>
       <c r="T18" s="6">
-        <v>9.571536</v>
+        <v>10.988352000000001</v>
       </c>
       <c r="U18" s="6">
-        <v>7.0621919999999996</v>
+        <v>13.353984000000001</v>
       </c>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
@@ -2110,69 +2110,69 @@
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
     </row>
-    <row r="19" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="6">
-        <v>0</v>
+        <v>3.9306239999999999</v>
       </c>
       <c r="C19" s="6">
-        <v>0</v>
+        <v>2.5125120000000001</v>
       </c>
       <c r="D19" s="6">
-        <v>5.8573440000000003</v>
+        <v>5.8641120000000004</v>
       </c>
       <c r="E19" s="6">
-        <v>20.386800000000001</v>
+        <v>20.276351999999999</v>
       </c>
       <c r="F19" s="6">
-        <v>155.315088</v>
+        <v>153.722736</v>
       </c>
       <c r="G19" s="6">
-        <v>452.15697599999999</v>
+        <v>473.20344000000006</v>
       </c>
       <c r="H19" s="6">
-        <v>138.77884800000001</v>
+        <v>138.15360000000001</v>
       </c>
       <c r="I19" s="6">
-        <v>119.35353600000001</v>
+        <v>122.762304</v>
       </c>
       <c r="J19" s="6">
-        <v>17.897615999999999</v>
+        <v>17.847935999999997</v>
       </c>
       <c r="K19" s="6">
-        <v>3727.4868000000001</v>
+        <v>3087.01008</v>
       </c>
       <c r="L19" s="6">
-        <v>15.20856</v>
+        <v>16.056432000000001</v>
       </c>
       <c r="M19" s="6">
-        <v>25.100928</v>
+        <v>0.65505600000000008</v>
       </c>
       <c r="N19" s="6">
-        <v>0</v>
+        <v>5.9039999999999995E-3</v>
       </c>
       <c r="O19" s="6">
-        <v>0.49276800000000004</v>
+        <v>0.49651200000000001</v>
       </c>
       <c r="P19" s="6">
-        <v>1513.753344</v>
+        <v>1509.6317759999999</v>
       </c>
       <c r="Q19" s="6">
-        <v>1406.3263199999999</v>
+        <v>1403.429472</v>
       </c>
       <c r="R19" s="6">
-        <v>592.72775999999999</v>
+        <v>1233.3474720000002</v>
       </c>
       <c r="S19" s="6">
-        <v>65.072592</v>
+        <v>66.321792000000002</v>
       </c>
       <c r="T19" s="6">
-        <v>1.9608479999999999</v>
+        <v>1.9663200000000001</v>
       </c>
       <c r="U19" s="6">
-        <v>5.7360959999999999</v>
+        <v>6.7265280000000001</v>
       </c>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
@@ -2193,69 +2193,69 @@
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
     </row>
-    <row r="20" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="6">
-        <v>0.28267199999999998</v>
+        <v>38.513663999999999</v>
       </c>
       <c r="C20" s="6">
-        <v>0</v>
+        <v>23.571360000000002</v>
       </c>
       <c r="D20" s="6">
-        <v>0</v>
+        <v>1.1790719999999999</v>
       </c>
       <c r="E20" s="6">
-        <v>34.404336000000001</v>
+        <v>32.431103999999998</v>
       </c>
       <c r="F20" s="6">
-        <v>157.25073600000002</v>
+        <v>147.25396799999999</v>
       </c>
       <c r="G20" s="6">
-        <v>86.115168000000011</v>
+        <v>84.145104000000003</v>
       </c>
       <c r="H20" s="6">
-        <v>395.49312000000003</v>
+        <v>390.29615999999999</v>
       </c>
       <c r="I20" s="6">
-        <v>488.70460800000001</v>
+        <v>486.59688</v>
       </c>
       <c r="J20" s="6">
-        <v>8.7194880000000001</v>
+        <v>8.4587039999999991</v>
       </c>
       <c r="K20" s="6">
-        <v>83.890512000000001</v>
+        <v>62.071199999999997</v>
       </c>
       <c r="L20" s="6">
-        <v>0</v>
+        <v>25.845696</v>
       </c>
       <c r="M20" s="6">
-        <v>44.324928</v>
+        <v>38.070720000000001</v>
       </c>
       <c r="N20" s="6">
-        <v>0</v>
+        <v>3.5428319999999998</v>
       </c>
       <c r="O20" s="6">
-        <v>8.7552000000000005E-2</v>
+        <v>8.7120000000000003E-2</v>
       </c>
       <c r="P20" s="6">
-        <v>945.33695999999998</v>
+        <v>906.20150399999989</v>
       </c>
       <c r="Q20" s="6">
-        <v>702.96407999999997</v>
+        <v>679.42900799999995</v>
       </c>
       <c r="R20" s="6">
-        <v>388.21017599999999</v>
+        <v>382.295232</v>
       </c>
       <c r="S20" s="6">
-        <v>104.629248</v>
+        <v>109.03737599999999</v>
       </c>
       <c r="T20" s="6">
-        <v>9.6088320000000014</v>
+        <v>20.127455999999999</v>
       </c>
       <c r="U20" s="6">
-        <v>2.8247040000000001</v>
+        <v>13.686623999999998</v>
       </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
@@ -2276,69 +2276,69 @@
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
     </row>
-    <row r="21" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="6">
-        <v>2.5205759999999997</v>
+        <v>10.07136</v>
       </c>
       <c r="C21" s="6">
-        <v>0.37180799999999997</v>
+        <v>4.8055680000000001</v>
       </c>
       <c r="D21" s="6">
-        <v>0</v>
+        <v>0.500112</v>
       </c>
       <c r="E21" s="6">
-        <v>13.537007999999998</v>
+        <v>12.328704</v>
       </c>
       <c r="F21" s="6">
-        <v>198.94391999999999</v>
+        <v>185.39265600000002</v>
       </c>
       <c r="G21" s="6">
-        <v>103.737888</v>
+        <v>99.774143999999993</v>
       </c>
       <c r="H21" s="6">
-        <v>672.41707199999996</v>
+        <v>667.17864000000009</v>
       </c>
       <c r="I21" s="6">
-        <v>729.22003200000006</v>
+        <v>736.83619199999998</v>
       </c>
       <c r="J21" s="6">
-        <v>106.51708799999999</v>
+        <v>97.342271999999994</v>
       </c>
       <c r="K21" s="6">
-        <v>49.331232</v>
+        <v>47.790576000000001</v>
       </c>
       <c r="L21" s="6">
-        <v>75.567887999999996</v>
+        <v>78.644159999999999</v>
       </c>
       <c r="M21" s="6">
-        <v>4.4616959999999999</v>
+        <v>4.3112159999999999</v>
       </c>
       <c r="N21" s="6">
-        <v>0</v>
+        <v>0.37036799999999998</v>
       </c>
       <c r="O21" s="6">
-        <v>0.10224</v>
+        <v>7.4880000000000002E-2</v>
       </c>
       <c r="P21" s="6">
-        <v>117.10771200000001</v>
+        <v>108.964224</v>
       </c>
       <c r="Q21" s="6">
-        <v>134.50046399999999</v>
+        <v>130.82126399999999</v>
       </c>
       <c r="R21" s="6">
-        <v>189.92591999999999</v>
+        <v>185.36328</v>
       </c>
       <c r="S21" s="6">
-        <v>55.843056000000004</v>
+        <v>73.123199999999997</v>
       </c>
       <c r="T21" s="6">
-        <v>31.606847999999999</v>
+        <v>32.430671999999994</v>
       </c>
       <c r="U21" s="6">
-        <v>8.5639679999999991</v>
+        <v>18.151631999999999</v>
       </c>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
@@ -2359,42 +2359,42 @@
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
     </row>
-    <row r="22" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="6">
-        <v>6.0153120000000007</v>
+        <v>10.792224000000001</v>
       </c>
       <c r="C22" s="6">
-        <v>2.05416</v>
+        <v>5.9643360000000003</v>
       </c>
       <c r="D22" s="6">
-        <v>0</v>
+        <v>0.91007999999999989</v>
       </c>
       <c r="E22" s="6">
-        <v>13.994064000000002</v>
+        <v>13.074479999999999</v>
       </c>
       <c r="F22" s="6">
-        <v>487.23091199999999</v>
+        <v>460.86408</v>
       </c>
       <c r="G22" s="6">
-        <v>116.94830400000001</v>
+        <v>113.40662399999999</v>
       </c>
       <c r="H22" s="6">
-        <v>1458.9567359999999</v>
+        <v>1443.21624</v>
       </c>
       <c r="I22" s="6">
-        <v>1268.5534560000001</v>
+        <v>1269.4152960000001</v>
       </c>
       <c r="J22" s="6">
-        <v>0</v>
+        <v>6.6528000000000004E-2</v>
       </c>
       <c r="K22" s="6">
-        <v>45.559584000000001</v>
+        <v>47.809440000000002</v>
       </c>
       <c r="L22" s="6">
-        <v>0</v>
+        <v>0.99619199999999997</v>
       </c>
       <c r="M22" s="6">
         <v>0</v>
@@ -2403,25 +2403,25 @@
         <v>0</v>
       </c>
       <c r="O22" s="6">
-        <v>6.4532160000000003</v>
+        <v>6.442704</v>
       </c>
       <c r="P22" s="6">
-        <v>143.88969599999999</v>
+        <v>138.808368</v>
       </c>
       <c r="Q22" s="6">
-        <v>367.57353599999999</v>
+        <v>363.100752</v>
       </c>
       <c r="R22" s="6">
-        <v>229.01875200000001</v>
+        <v>224.16321600000001</v>
       </c>
       <c r="S22" s="6">
-        <v>151.52644799999999</v>
+        <v>183.17044799999999</v>
       </c>
       <c r="T22" s="6">
-        <v>132.859872</v>
+        <v>133.410528</v>
       </c>
       <c r="U22" s="6">
-        <v>31.208112</v>
+        <v>46.232928000000001</v>
       </c>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
@@ -2442,69 +2442,69 @@
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
     </row>
-    <row r="23" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="6">
-        <v>0</v>
+        <v>40.606559999999995</v>
       </c>
       <c r="C23" s="6">
-        <v>0</v>
+        <v>32.191344000000001</v>
       </c>
       <c r="D23" s="6">
-        <v>0</v>
+        <v>1.033776</v>
       </c>
       <c r="E23" s="6">
-        <v>16.006751999999999</v>
+        <v>14.909904000000001</v>
       </c>
       <c r="F23" s="6">
-        <v>214.72819199999998</v>
+        <v>200.05848</v>
       </c>
       <c r="G23" s="6">
-        <v>106.16385600000001</v>
+        <v>104.281488</v>
       </c>
       <c r="H23" s="6">
-        <v>677.26036799999997</v>
+        <v>666.57225599999992</v>
       </c>
       <c r="I23" s="6">
-        <v>603.74952000000008</v>
+        <v>601.02849600000002</v>
       </c>
       <c r="J23" s="6">
-        <v>287.55849599999999</v>
+        <v>283.26369599999998</v>
       </c>
       <c r="K23" s="6">
-        <v>406.681488</v>
+        <v>374.12495999999999</v>
       </c>
       <c r="L23" s="6">
-        <v>0</v>
+        <v>35.819712000000003</v>
       </c>
       <c r="M23" s="6">
-        <v>2.46888</v>
+        <v>1.8970560000000001</v>
       </c>
       <c r="N23" s="6">
-        <v>0</v>
+        <v>0.21873600000000001</v>
       </c>
       <c r="O23" s="6">
-        <v>0.23443200000000003</v>
+        <v>0.23025599999999999</v>
       </c>
       <c r="P23" s="6">
-        <v>1599.48</v>
+        <v>1558.4081759999999</v>
       </c>
       <c r="Q23" s="6">
-        <v>1552.7952</v>
+        <v>1521.925776</v>
       </c>
       <c r="R23" s="6">
-        <v>548.99899200000004</v>
+        <v>543.98966399999995</v>
       </c>
       <c r="S23" s="6">
-        <v>107.35070400000001</v>
+        <v>123.80515200000001</v>
       </c>
       <c r="T23" s="6">
-        <v>18.828144000000002</v>
+        <v>24.234767999999999</v>
       </c>
       <c r="U23" s="6">
-        <v>12.575376</v>
+        <v>26.399087999999999</v>
       </c>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
@@ -2525,42 +2525,42 @@
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
     </row>
-    <row r="24" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="6">
-        <v>1.203552</v>
+        <v>7.2048960000000006</v>
       </c>
       <c r="C24" s="6">
-        <v>0.97056000000000009</v>
+        <v>3.4515359999999999</v>
       </c>
       <c r="D24" s="6">
-        <v>0</v>
+        <v>0.17452799999999999</v>
       </c>
       <c r="E24" s="6">
-        <v>10.588464</v>
+        <v>10.039680000000001</v>
       </c>
       <c r="F24" s="6">
-        <v>99.195119999999989</v>
+        <v>92.679407999999995</v>
       </c>
       <c r="G24" s="6">
-        <v>10.977839999999999</v>
+        <v>10.559088000000001</v>
       </c>
       <c r="H24" s="6">
-        <v>285.90465599999999</v>
+        <v>281.78294399999999</v>
       </c>
       <c r="I24" s="6">
-        <v>293.78289599999999</v>
+        <v>293.01825600000001</v>
       </c>
       <c r="J24" s="6">
-        <v>27.236303999999997</v>
+        <v>25.944768</v>
       </c>
       <c r="K24" s="6">
-        <v>88.139231999999993</v>
+        <v>84.433968000000007</v>
       </c>
       <c r="L24" s="6">
-        <v>0</v>
+        <v>4.7671199999999994</v>
       </c>
       <c r="M24" s="6">
         <v>0</v>
@@ -2572,22 +2572,22 @@
         <v>0</v>
       </c>
       <c r="P24" s="6">
-        <v>283.04568</v>
+        <v>276.61982399999999</v>
       </c>
       <c r="Q24" s="6">
-        <v>331.85851200000002</v>
+        <v>330.37660800000003</v>
       </c>
       <c r="R24" s="6">
-        <v>77.592240000000004</v>
+        <v>75.429648</v>
       </c>
       <c r="S24" s="6">
-        <v>51.261839999999999</v>
+        <v>59.932368000000004</v>
       </c>
       <c r="T24" s="6">
-        <v>8.5220640000000003</v>
+        <v>9.5708160000000007</v>
       </c>
       <c r="U24" s="6">
-        <v>7.3483199999999993</v>
+        <v>11.634335999999999</v>
       </c>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
@@ -2608,42 +2608,42 @@
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
     </row>
-    <row r="25" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="6">
-        <v>0.80164799999999992</v>
+        <v>1.9869119999999998</v>
       </c>
       <c r="C25" s="6">
-        <v>1.413216</v>
+        <v>2.229552</v>
       </c>
       <c r="D25" s="6">
-        <v>0</v>
+        <v>0.11174400000000001</v>
       </c>
       <c r="E25" s="6">
-        <v>2.297088</v>
+        <v>2.0272320000000001</v>
       </c>
       <c r="F25" s="6">
-        <v>86.67676800000001</v>
+        <v>81.601919999999993</v>
       </c>
       <c r="G25" s="6">
-        <v>7.4891520000000007</v>
+        <v>7.1467199999999993</v>
       </c>
       <c r="H25" s="6">
-        <v>275.23641600000002</v>
+        <v>271.63828799999999</v>
       </c>
       <c r="I25" s="6">
-        <v>241.81732799999997</v>
+        <v>241.64856</v>
       </c>
       <c r="J25" s="6">
-        <v>0</v>
+        <v>2.2175999999999998E-2</v>
       </c>
       <c r="K25" s="6">
-        <v>3.9634559999999999</v>
+        <v>4.1149440000000004</v>
       </c>
       <c r="L25" s="6">
-        <v>0</v>
+        <v>0.15436800000000001</v>
       </c>
       <c r="M25" s="6">
         <v>0</v>
@@ -2655,22 +2655,22 @@
         <v>0</v>
       </c>
       <c r="P25" s="6">
-        <v>38.869487999999997</v>
+        <v>37.637423999999996</v>
       </c>
       <c r="Q25" s="6">
-        <v>80.806319999999999</v>
+        <v>79.938143999999994</v>
       </c>
       <c r="R25" s="6">
-        <v>47.496959999999994</v>
+        <v>46.364111999999999</v>
       </c>
       <c r="S25" s="6">
-        <v>27.079343999999999</v>
+        <v>33.805296000000006</v>
       </c>
       <c r="T25" s="6">
-        <v>10.119024000000001</v>
+        <v>10.511856</v>
       </c>
       <c r="U25" s="6">
-        <v>2.8729439999999999</v>
+        <v>5.9986079999999999</v>
       </c>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
@@ -2691,69 +2691,69 @@
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
     </row>
-    <row r="26" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="6">
-        <v>1.5438240000000001</v>
+        <v>111.591792</v>
       </c>
       <c r="C26" s="6">
-        <v>1.538208</v>
+        <v>118.53863999999999</v>
       </c>
       <c r="D26" s="6">
-        <v>13.488335999999999</v>
+        <v>14.889888000000001</v>
       </c>
       <c r="E26" s="6">
-        <v>418.577472</v>
+        <v>400.41302400000001</v>
       </c>
       <c r="F26" s="6">
-        <v>830.08886399999994</v>
+        <v>797.76417600000002</v>
       </c>
       <c r="G26" s="6">
-        <v>2047.1958719999998</v>
+        <v>2034.8624159999999</v>
       </c>
       <c r="H26" s="6">
-        <v>1652.2090560000001</v>
+        <v>1636.1896320000001</v>
       </c>
       <c r="I26" s="6">
-        <v>2693.5598879999998</v>
+        <v>2795.5759680000001</v>
       </c>
       <c r="J26" s="6">
-        <v>2702.091312</v>
+        <v>2604.96648</v>
       </c>
       <c r="K26" s="6">
-        <v>3402.4016159999996</v>
+        <v>2747.1327839999999</v>
       </c>
       <c r="L26" s="6">
-        <v>99.96696</v>
+        <v>171.14083200000002</v>
       </c>
       <c r="M26" s="6">
-        <v>769.44297599999993</v>
+        <v>722.19960000000003</v>
       </c>
       <c r="N26" s="6">
-        <v>158.41152</v>
+        <v>162.98438400000001</v>
       </c>
       <c r="O26" s="6">
-        <v>36.691488</v>
+        <v>36.399887999999997</v>
       </c>
       <c r="P26" s="6">
-        <v>4216.9350240000003</v>
+        <v>4097.0891520000005</v>
       </c>
       <c r="Q26" s="6">
-        <v>3953.2934880000003</v>
+        <v>3867.0942240000004</v>
       </c>
       <c r="R26" s="6">
-        <v>2695.6943999999999</v>
+        <v>3261.8174399999998</v>
       </c>
       <c r="S26" s="6">
-        <v>414.32428799999997</v>
+        <v>470.69639999999998</v>
       </c>
       <c r="T26" s="6">
-        <v>47.077632000000001</v>
+        <v>58.709952000000001</v>
       </c>
       <c r="U26" s="6">
-        <v>29.239776000000003</v>
+        <v>73.783152000000001</v>
       </c>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
@@ -2774,69 +2774,69 @@
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
     </row>
-    <row r="27" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="6">
-        <v>0</v>
+        <v>24.500015999999999</v>
       </c>
       <c r="C27" s="6">
-        <v>0</v>
+        <v>26.510832000000001</v>
       </c>
       <c r="D27" s="6">
-        <v>1.216656</v>
+        <v>2.128752</v>
       </c>
       <c r="E27" s="6">
-        <v>52.002720000000004</v>
+        <v>50.130288</v>
       </c>
       <c r="F27" s="6">
-        <v>107.005824</v>
+        <v>101.72188800000001</v>
       </c>
       <c r="G27" s="6">
-        <v>404.72510399999999</v>
+        <v>401.27760000000001</v>
       </c>
       <c r="H27" s="6">
-        <v>202.57488000000001</v>
+        <v>198.777456</v>
       </c>
       <c r="I27" s="6">
-        <v>157.47408000000001</v>
+        <v>158.40014399999998</v>
       </c>
       <c r="J27" s="6">
-        <v>860.95627200000001</v>
+        <v>842.39064000000008</v>
       </c>
       <c r="K27" s="6">
-        <v>486.32112000000001</v>
+        <v>465.08702400000004</v>
       </c>
       <c r="L27" s="6">
-        <v>12.815856</v>
+        <v>37.718063999999998</v>
       </c>
       <c r="M27" s="6">
-        <v>145.90670399999999</v>
+        <v>136.92671999999999</v>
       </c>
       <c r="N27" s="6">
-        <v>18.31392</v>
+        <v>23.301359999999999</v>
       </c>
       <c r="O27" s="6">
-        <v>1.1593440000000002</v>
+        <v>0.78048000000000006</v>
       </c>
       <c r="P27" s="6">
-        <v>1001.028672</v>
+        <v>976.3938720000001</v>
       </c>
       <c r="Q27" s="6">
-        <v>1173.440736</v>
+        <v>1161.5384160000001</v>
       </c>
       <c r="R27" s="6">
-        <v>494.04772800000001</v>
+        <v>488.09217599999999</v>
       </c>
       <c r="S27" s="6">
-        <v>35.264448000000002</v>
+        <v>43.861536000000001</v>
       </c>
       <c r="T27" s="6">
-        <v>4.1235839999999993</v>
+        <v>9.4982399999999991</v>
       </c>
       <c r="U27" s="6">
-        <v>5.5689120000000001</v>
+        <v>14.938272</v>
       </c>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
@@ -2857,69 +2857,69 @@
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
     </row>
-    <row r="28" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="6">
-        <v>3.6308160000000003</v>
+        <v>29.509056000000001</v>
       </c>
       <c r="C28" s="6">
-        <v>0.44107200000000002</v>
+        <v>11.246112</v>
       </c>
       <c r="D28" s="6">
-        <v>0</v>
+        <v>0.41731200000000002</v>
       </c>
       <c r="E28" s="6">
-        <v>44.598240000000004</v>
+        <v>42.590447999999995</v>
       </c>
       <c r="F28" s="6">
-        <v>124.6932</v>
+        <v>115.85476799999999</v>
       </c>
       <c r="G28" s="6">
-        <v>65.296368000000001</v>
+        <v>65.37312</v>
       </c>
       <c r="H28" s="6">
-        <v>295.73611199999999</v>
+        <v>288.764928</v>
       </c>
       <c r="I28" s="6">
-        <v>396.682704</v>
+        <v>402.73127999999997</v>
       </c>
       <c r="J28" s="6">
-        <v>529.09185600000001</v>
+        <v>505.63512000000003</v>
       </c>
       <c r="K28" s="6">
-        <v>100.843632</v>
+        <v>84.442176000000003</v>
       </c>
       <c r="L28" s="6">
-        <v>2.325024</v>
+        <v>21.531168000000001</v>
       </c>
       <c r="M28" s="6">
-        <v>29.602656</v>
+        <v>26.054207999999999</v>
       </c>
       <c r="N28" s="6">
-        <v>3.9003839999999999</v>
+        <v>5.0207040000000003</v>
       </c>
       <c r="O28" s="6">
         <v>0</v>
       </c>
       <c r="P28" s="6">
-        <v>166.259376</v>
+        <v>140.04187199999998</v>
       </c>
       <c r="Q28" s="6">
-        <v>295.49520000000001</v>
+        <v>299.89771200000001</v>
       </c>
       <c r="R28" s="6">
-        <v>419.50094400000006</v>
+        <v>412.39396800000003</v>
       </c>
       <c r="S28" s="6">
-        <v>49.461264</v>
+        <v>58.634064000000002</v>
       </c>
       <c r="T28" s="6">
-        <v>6.2298720000000003</v>
+        <v>14.348448000000001</v>
       </c>
       <c r="U28" s="6">
-        <v>5.9234400000000003</v>
+        <v>15.216623999999999</v>
       </c>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
@@ -2940,69 +2940,69 @@
       <c r="AM28" s="1"/>
       <c r="AN28" s="1"/>
     </row>
-    <row r="29" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="6">
-        <v>0</v>
+        <v>4.1672160000000007</v>
       </c>
       <c r="C29" s="6">
-        <v>0.46296000000000004</v>
+        <v>2.1680639999999998</v>
       </c>
       <c r="D29" s="6">
-        <v>0</v>
+        <v>0.17668800000000001</v>
       </c>
       <c r="E29" s="6">
-        <v>9.5813279999999992</v>
+        <v>8.8482240000000001</v>
       </c>
       <c r="F29" s="6">
-        <v>44.889696000000001</v>
+        <v>41.019264</v>
       </c>
       <c r="G29" s="6">
-        <v>5.9758559999999994</v>
+        <v>5.8252319999999997</v>
       </c>
       <c r="H29" s="6">
-        <v>132.65568000000002</v>
+        <v>131.76619199999999</v>
       </c>
       <c r="I29" s="6">
-        <v>214.83892799999998</v>
+        <v>220.50863999999999</v>
       </c>
       <c r="J29" s="6">
-        <v>21.004848000000003</v>
+        <v>18.726623999999997</v>
       </c>
       <c r="K29" s="6">
-        <v>13.932</v>
+        <v>12.382703999999999</v>
       </c>
       <c r="L29" s="6">
-        <v>0.69998400000000005</v>
+        <v>2.6402400000000004</v>
       </c>
       <c r="M29" s="6">
-        <v>32.11992</v>
+        <v>25.323119999999999</v>
       </c>
       <c r="N29" s="6">
-        <v>0</v>
+        <v>0.48283199999999998</v>
       </c>
       <c r="O29" s="6">
-        <v>0.40348800000000001</v>
+        <v>0.23990400000000001</v>
       </c>
       <c r="P29" s="6">
-        <v>54.893807999999993</v>
+        <v>50.583024000000002</v>
       </c>
       <c r="Q29" s="6">
-        <v>43.979040000000005</v>
+        <v>43.165728000000001</v>
       </c>
       <c r="R29" s="6">
-        <v>70.999487999999999</v>
+        <v>68.50281600000001</v>
       </c>
       <c r="S29" s="6">
-        <v>22.562784000000001</v>
+        <v>28.635120000000001</v>
       </c>
       <c r="T29" s="6">
-        <v>3.3012000000000001</v>
+        <v>4.1549760000000004</v>
       </c>
       <c r="U29" s="6">
-        <v>2.488896</v>
+        <v>5.4812160000000008</v>
       </c>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
@@ -3023,69 +3023,69 @@
       <c r="AM29" s="1"/>
       <c r="AN29" s="1"/>
     </row>
-    <row r="30" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="6">
-        <v>0</v>
+        <v>25.120656</v>
       </c>
       <c r="C30" s="6">
-        <v>0</v>
+        <v>14.516639999999999</v>
       </c>
       <c r="D30" s="6">
-        <v>0</v>
+        <v>0.81590399999999996</v>
       </c>
       <c r="E30" s="6">
-        <v>125.681184</v>
+        <v>117.82656000000001</v>
       </c>
       <c r="F30" s="6">
-        <v>108.659952</v>
+        <v>98.735184000000004</v>
       </c>
       <c r="G30" s="6">
-        <v>220.74696</v>
+        <v>217.54944</v>
       </c>
       <c r="H30" s="6">
-        <v>264.284784</v>
+        <v>254.88302400000003</v>
       </c>
       <c r="I30" s="6">
-        <v>224.01388799999998</v>
+        <v>236.91067200000003</v>
       </c>
       <c r="J30" s="6">
-        <v>400.67049600000001</v>
+        <v>375.16463999999996</v>
       </c>
       <c r="K30" s="6">
-        <v>652.24944000000005</v>
+        <v>617.37724800000001</v>
       </c>
       <c r="L30" s="6">
-        <v>0.80222399999999994</v>
+        <v>38.561040000000006</v>
       </c>
       <c r="M30" s="6">
-        <v>10.166544</v>
+        <v>9.0442079999999994</v>
       </c>
       <c r="N30" s="6">
-        <v>4.1844960000000002</v>
+        <v>4.2228000000000003</v>
       </c>
       <c r="O30" s="6">
-        <v>1.6375680000000001</v>
+        <v>1.562832</v>
       </c>
       <c r="P30" s="6">
-        <v>1375.7035679999999</v>
+        <v>1350.3968640000001</v>
       </c>
       <c r="Q30" s="6">
-        <v>828.37872000000004</v>
+        <v>833.99428799999998</v>
       </c>
       <c r="R30" s="6">
-        <v>560.49393600000008</v>
+        <v>554.68468799999994</v>
       </c>
       <c r="S30" s="6">
-        <v>29.963664000000001</v>
+        <v>47.089872</v>
       </c>
       <c r="T30" s="6">
-        <v>5.3998559999999998</v>
+        <v>7.9097759999999999</v>
       </c>
       <c r="U30" s="6">
-        <v>3.8878559999999998</v>
+        <v>10.589039999999999</v>
       </c>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
@@ -3106,69 +3106,69 @@
       <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
     </row>
-    <row r="31" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="6">
-        <v>0</v>
+        <v>39.276288000000001</v>
       </c>
       <c r="C31" s="6">
-        <v>0</v>
+        <v>19.001376</v>
       </c>
       <c r="D31" s="6">
-        <v>4.5440639999999997</v>
+        <v>5.5481759999999998</v>
       </c>
       <c r="E31" s="6">
-        <v>83.412000000000006</v>
+        <v>80.828640000000007</v>
       </c>
       <c r="F31" s="6">
-        <v>104.232816</v>
+        <v>94.270895999999993</v>
       </c>
       <c r="G31" s="6">
-        <v>247.94164799999999</v>
+        <v>244.32681600000001</v>
       </c>
       <c r="H31" s="6">
-        <v>235.39420800000002</v>
+        <v>230.05727999999999</v>
       </c>
       <c r="I31" s="6">
-        <v>186.92308799999998</v>
+        <v>188.87832</v>
       </c>
       <c r="J31" s="6">
-        <v>582.761664</v>
+        <v>566.45236799999998</v>
       </c>
       <c r="K31" s="6">
-        <v>716.35867199999996</v>
+        <v>686.91067199999998</v>
       </c>
       <c r="L31" s="6">
-        <v>17.357327999999999</v>
+        <v>50.451696000000005</v>
       </c>
       <c r="M31" s="6">
-        <v>51.256079999999997</v>
+        <v>49.120272</v>
       </c>
       <c r="N31" s="6">
-        <v>53.6616</v>
+        <v>55.062288000000002</v>
       </c>
       <c r="O31" s="6">
-        <v>1.6813439999999999</v>
+        <v>1.675152</v>
       </c>
       <c r="P31" s="6">
-        <v>2002.4913600000002</v>
+        <v>1962.878256</v>
       </c>
       <c r="Q31" s="6">
-        <v>890.93764800000008</v>
+        <v>882.32284800000002</v>
       </c>
       <c r="R31" s="6">
-        <v>348.196032</v>
+        <v>343.06142400000004</v>
       </c>
       <c r="S31" s="6">
-        <v>45.006624000000002</v>
+        <v>58.746816000000003</v>
       </c>
       <c r="T31" s="6">
-        <v>7.2944639999999996</v>
+        <v>13.413167999999999</v>
       </c>
       <c r="U31" s="6">
-        <v>4.966272</v>
+        <v>12.075407999999999</v>
       </c>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
@@ -3189,69 +3189,69 @@
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
     </row>
-    <row r="32" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="6">
-        <v>6.5664E-2</v>
+        <v>32.100335999999999</v>
       </c>
       <c r="C32" s="6">
-        <v>0</v>
+        <v>16.688016000000001</v>
       </c>
       <c r="D32" s="6">
-        <v>78.040080000000003</v>
+        <v>77.798591999999999</v>
       </c>
       <c r="E32" s="6">
-        <v>122.90457600000001</v>
+        <v>121.75833600000001</v>
       </c>
       <c r="F32" s="6">
-        <v>376.567632</v>
+        <v>358.87795199999999</v>
       </c>
       <c r="G32" s="6">
-        <v>1021.9739039999999</v>
+        <v>1013.50368</v>
       </c>
       <c r="H32" s="6">
-        <v>902.50113599999997</v>
+        <v>899.22902399999998</v>
       </c>
       <c r="I32" s="6">
-        <v>1100.500272</v>
+        <v>1136.3784479999999</v>
       </c>
       <c r="J32" s="6">
-        <v>31.375440000000001</v>
+        <v>28.675440000000002</v>
       </c>
       <c r="K32" s="6">
-        <v>3124.9968480000002</v>
+        <v>2928.721536</v>
       </c>
       <c r="L32" s="6">
-        <v>1.25928</v>
+        <v>203.73148799999998</v>
       </c>
       <c r="M32" s="6">
-        <v>947.84975999999995</v>
+        <v>932.39755199999991</v>
       </c>
       <c r="N32" s="6">
-        <v>29.006928000000002</v>
+        <v>29.752847999999997</v>
       </c>
       <c r="O32" s="6">
-        <v>11.695824</v>
+        <v>11.480399999999999</v>
       </c>
       <c r="P32" s="6">
-        <v>5240.0305440000002</v>
+        <v>5214.157776</v>
       </c>
       <c r="Q32" s="6">
-        <v>3677.7823200000003</v>
+        <v>3660.4239840000005</v>
       </c>
       <c r="R32" s="6">
-        <v>2150.1967679999998</v>
+        <v>2132.538192</v>
       </c>
       <c r="S32" s="6">
-        <v>277.44969600000002</v>
+        <v>287.50939199999999</v>
       </c>
       <c r="T32" s="6">
-        <v>62.122895999999997</v>
+        <v>62.735040000000005</v>
       </c>
       <c r="U32" s="6">
-        <v>20.059055999999998</v>
+        <v>28.280159999999999</v>
       </c>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
@@ -3272,7 +3272,8 @@
       <c r="AM32" s="1"/>
       <c r="AN32" s="1"/>
     </row>
-    <row r="33" s="5" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="33" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3280,24 +3281,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7092D54C-53F0-45DD-9FD7-B6FB69205D33}">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="15.08984375" customWidth="1"/>
-    <col min="7" max="8" width="14.1796875" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" customWidth="1"/>
-    <col min="15" max="16" width="14.1796875" customWidth="1"/>
-    <col min="17" max="17" width="14.54296875" customWidth="1"/>
-    <col min="20" max="20" width="14.1796875" customWidth="1"/>
-    <col min="21" max="21" width="16.6328125" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="8" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
+    <col min="15" max="16" width="14.21875" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" customWidth="1"/>
+    <col min="20" max="20" width="14.21875" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -3362,432 +3363,432 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="6">
-        <v>0</v>
+        <v>3.7159199999999997</v>
       </c>
       <c r="C2" s="6">
-        <v>0</v>
+        <v>2.3267519999999999</v>
       </c>
       <c r="D2" s="6">
-        <v>5.8573440000000003</v>
+        <v>5.8641120000000004</v>
       </c>
       <c r="E2" s="6">
-        <v>19.305648000000001</v>
+        <v>19.195488000000001</v>
       </c>
       <c r="F2" s="6">
-        <v>151.17004800000001</v>
+        <v>149.58000000000001</v>
       </c>
       <c r="G2" s="6">
-        <v>447.019632</v>
+        <v>468.02404800000005</v>
       </c>
       <c r="H2" s="6">
-        <v>137.91787199999999</v>
+        <v>137.29032000000001</v>
       </c>
       <c r="I2" s="6">
-        <v>119.01383999999999</v>
+        <v>122.42001599999999</v>
       </c>
       <c r="J2" s="6">
-        <v>20.359728</v>
+        <v>20.309616000000002</v>
       </c>
       <c r="K2" s="6">
-        <v>3166.710912</v>
+        <v>2544.47136</v>
       </c>
       <c r="L2" s="6">
-        <v>15.20856</v>
+        <v>15.946848000000001</v>
       </c>
       <c r="M2" s="6">
-        <v>25.100928</v>
+        <v>0.65505600000000008</v>
       </c>
       <c r="N2" s="6">
-        <v>0</v>
+        <v>5.9039999999999995E-3</v>
       </c>
       <c r="O2" s="6">
-        <v>0.49276800000000004</v>
+        <v>0.49651200000000001</v>
       </c>
       <c r="P2" s="6">
-        <v>1375.141392</v>
+        <v>1371.1920480000001</v>
       </c>
       <c r="Q2" s="6">
-        <v>1223.749728</v>
+        <v>1221.078528</v>
       </c>
       <c r="R2" s="6">
-        <v>588.38515199999995</v>
+        <v>1210.755312</v>
       </c>
       <c r="S2" s="6">
-        <v>64.121759999999995</v>
+        <v>65.373407999999998</v>
       </c>
       <c r="T2" s="6">
-        <v>1.9598400000000002</v>
+        <v>1.9657439999999999</v>
       </c>
       <c r="U2" s="6">
-        <v>6.1372800000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+        <v>7.1282880000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="6">
-        <v>0.622224</v>
+        <v>4.0380480000000007</v>
       </c>
       <c r="C3" s="6">
-        <v>0</v>
+        <v>1.8764639999999999</v>
       </c>
       <c r="D3" s="6">
-        <v>0</v>
+        <v>7.92E-3</v>
       </c>
       <c r="E3" s="6">
-        <v>41.202143999999997</v>
+        <v>40.731120000000004</v>
       </c>
       <c r="F3" s="6">
-        <v>26.588159999999998</v>
+        <v>26.152415999999999</v>
       </c>
       <c r="G3" s="6">
-        <v>29.345615999999996</v>
+        <v>29.036303999999998</v>
       </c>
       <c r="H3" s="6">
-        <v>43.075296000000002</v>
+        <v>42.545088</v>
       </c>
       <c r="I3" s="6">
-        <v>43.968384</v>
+        <v>45.267552000000002</v>
       </c>
       <c r="J3" s="6">
-        <v>18.121824</v>
+        <v>16.95168</v>
       </c>
       <c r="K3" s="6">
-        <v>520.80912000000001</v>
+        <v>521.972352</v>
       </c>
       <c r="L3" s="6">
-        <v>1.4057280000000001</v>
+        <v>2.2226400000000002</v>
       </c>
       <c r="M3" s="6">
-        <v>17.038224</v>
+        <v>17.044992000000001</v>
       </c>
       <c r="N3" s="6">
-        <v>4.6339199999999998</v>
+        <v>4.6330559999999998</v>
       </c>
       <c r="O3" s="6">
-        <v>0.45547200000000004</v>
+        <v>0.45475200000000005</v>
       </c>
       <c r="P3" s="6">
-        <v>584.72884800000008</v>
+        <v>581.11516799999993</v>
       </c>
       <c r="Q3" s="6">
-        <v>677.94739200000004</v>
+        <v>675.95112000000006</v>
       </c>
       <c r="R3" s="6">
-        <v>182.76019199999999</v>
+        <v>180.75441599999999</v>
       </c>
       <c r="S3" s="6">
-        <v>4.6599839999999997</v>
+        <v>6.0134400000000001</v>
       </c>
       <c r="T3" s="6">
-        <v>0.15868800000000002</v>
+        <v>0.19123199999999999</v>
       </c>
       <c r="U3" s="6">
-        <v>0.654192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+        <v>1.207584</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="6">
-        <v>0.184752</v>
+        <v>91.234511999999995</v>
       </c>
       <c r="C4" s="6">
-        <v>0</v>
+        <v>116.986896</v>
       </c>
       <c r="D4" s="6">
-        <v>3.5110080000000004</v>
+        <v>3.8666879999999999</v>
       </c>
       <c r="E4" s="6">
-        <v>195.55027200000001</v>
+        <v>186.80961600000001</v>
       </c>
       <c r="F4" s="6">
-        <v>367.84857599999998</v>
+        <v>356.88355200000001</v>
       </c>
       <c r="G4" s="6">
-        <v>1289.7100800000001</v>
+        <v>1292.5278720000001</v>
       </c>
       <c r="H4" s="6">
-        <v>598.49913600000002</v>
+        <v>593.97681599999999</v>
       </c>
       <c r="I4" s="6">
-        <v>1148.18112</v>
+        <v>1278.9503999999999</v>
       </c>
       <c r="J4" s="6">
-        <v>2102.441472</v>
+        <v>1967.59944</v>
       </c>
       <c r="K4" s="6">
-        <v>3119.3520480000002</v>
+        <v>2423.5806239999997</v>
       </c>
       <c r="L4" s="6">
-        <v>74.049552000000006</v>
+        <v>125.500176</v>
       </c>
       <c r="M4" s="6">
-        <v>761.05699200000004</v>
+        <v>747.886032</v>
       </c>
       <c r="N4" s="6">
-        <v>255.22732799999997</v>
+        <v>255.13876800000003</v>
       </c>
       <c r="O4" s="6">
-        <v>31.399343999999999</v>
+        <v>31.844591999999999</v>
       </c>
       <c r="P4" s="6">
-        <v>5572.0062719999996</v>
+        <v>5474.5162559999999</v>
       </c>
       <c r="Q4" s="6">
-        <v>4413.1302720000003</v>
+        <v>4318.2138240000004</v>
       </c>
       <c r="R4" s="6">
-        <v>2371.1572799999999</v>
+        <v>2995.5540960000003</v>
       </c>
       <c r="S4" s="6">
-        <v>194.38099199999999</v>
+        <v>214.70428799999999</v>
       </c>
       <c r="T4" s="6">
-        <v>10.560096000000001</v>
+        <v>15.027407999999999</v>
       </c>
       <c r="U4" s="6">
-        <v>10.482624000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+        <v>29.029968</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="6">
-        <v>0</v>
+        <v>30.634559999999997</v>
       </c>
       <c r="C5" s="6">
-        <v>0</v>
+        <v>19.547135999999998</v>
       </c>
       <c r="D5" s="6">
-        <v>80.883936000000006</v>
+        <v>80.501040000000003</v>
       </c>
       <c r="E5" s="6">
-        <v>137.065248</v>
+        <v>135.98366399999998</v>
       </c>
       <c r="F5" s="6">
-        <v>507.98995199999996</v>
+        <v>483.653232</v>
       </c>
       <c r="G5" s="6">
-        <v>1236.4416000000001</v>
+        <v>1227.7159199999999</v>
       </c>
       <c r="H5" s="6">
-        <v>1210.4311680000001</v>
+        <v>1204.142112</v>
       </c>
       <c r="I5" s="6">
-        <v>1434.6907199999998</v>
+        <v>1482.9376320000001</v>
       </c>
       <c r="J5" s="6">
-        <v>272.75817599999999</v>
+        <v>261.011664</v>
       </c>
       <c r="K5" s="6">
-        <v>3011.9181120000003</v>
+        <v>2783.9583360000001</v>
       </c>
       <c r="L5" s="6">
-        <v>15.867504</v>
+        <v>249.88507200000001</v>
       </c>
       <c r="M5" s="6">
-        <v>1079.85456</v>
+        <v>1060.021872</v>
       </c>
       <c r="N5" s="6">
-        <v>72.165599999999998</v>
+        <v>71.666495999999995</v>
       </c>
       <c r="O5" s="6">
-        <v>15.048432</v>
+        <v>14.837760000000001</v>
       </c>
       <c r="P5" s="6">
-        <v>2474.8708320000001</v>
+        <v>2452.5623519999999</v>
       </c>
       <c r="Q5" s="6">
-        <v>2180.8594079999998</v>
+        <v>2162.685888</v>
       </c>
       <c r="R5" s="6">
-        <v>2411.1996480000003</v>
+        <v>2391.9464160000002</v>
       </c>
       <c r="S5" s="6">
-        <v>374.738112</v>
+        <v>390.576528</v>
       </c>
       <c r="T5" s="6">
-        <v>63.081792000000007</v>
+        <v>63.413280000000007</v>
       </c>
       <c r="U5" s="6">
-        <v>25.263935999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+        <v>37.566144000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="6">
-        <v>7.3738080000000004</v>
+        <v>156.29731200000001</v>
       </c>
       <c r="C6" s="6">
-        <v>3.2447520000000001</v>
+        <v>100.18512</v>
       </c>
       <c r="D6" s="6">
-        <v>55.883952000000001</v>
+        <v>59.381568000000009</v>
       </c>
       <c r="E6" s="6">
-        <v>147.140784</v>
+        <v>141.63696000000002</v>
       </c>
       <c r="F6" s="6">
-        <v>808.2396</v>
+        <v>759.64075199999991</v>
       </c>
       <c r="G6" s="6">
-        <v>438.23375999999996</v>
+        <v>429.44140800000002</v>
       </c>
       <c r="H6" s="6">
-        <v>2288.3320800000001</v>
+        <v>2251.9823040000001</v>
       </c>
       <c r="I6" s="6">
-        <v>2170.8440639999999</v>
+        <v>2175.1917120000003</v>
       </c>
       <c r="J6" s="6">
-        <v>613.23393600000009</v>
+        <v>593.78702399999997</v>
       </c>
       <c r="K6" s="6">
-        <v>1571.1792480000001</v>
+        <v>1406.2847039999999</v>
       </c>
       <c r="L6" s="6">
-        <v>1.0159200000000002</v>
+        <v>181.769904</v>
       </c>
       <c r="M6" s="6">
-        <v>369.48326400000002</v>
+        <v>359.56036800000004</v>
       </c>
       <c r="N6" s="6">
-        <v>13.013856000000001</v>
+        <v>18.539567999999999</v>
       </c>
       <c r="O6" s="6">
-        <v>6.0539040000000002</v>
+        <v>6.0167519999999994</v>
       </c>
       <c r="P6" s="6">
-        <v>5763.4490880000003</v>
+        <v>5611.2850079999998</v>
       </c>
       <c r="Q6" s="6">
-        <v>5072.2208639999999</v>
+        <v>4980.2427360000001</v>
       </c>
       <c r="R6" s="6">
-        <v>1903.8054239999999</v>
+        <v>1882.4785920000002</v>
       </c>
       <c r="S6" s="6">
-        <v>408.68135999999998</v>
+        <v>458.38411200000002</v>
       </c>
       <c r="T6" s="6">
-        <v>113.45371200000001</v>
+        <v>137.76696000000001</v>
       </c>
       <c r="U6" s="6">
-        <v>37.038815999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+        <v>82.439568000000008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="6">
-        <v>3.4475039999999999</v>
+        <v>19.380960000000002</v>
       </c>
       <c r="C7" s="6">
-        <v>1.7092799999999999</v>
+        <v>9.5725440000000006</v>
       </c>
       <c r="D7" s="6">
-        <v>0</v>
+        <v>0.58435200000000009</v>
       </c>
       <c r="E7" s="6">
-        <v>39.289248000000001</v>
+        <v>37.903391999999997</v>
       </c>
       <c r="F7" s="6">
-        <v>373.67726400000004</v>
+        <v>352.88654400000001</v>
       </c>
       <c r="G7" s="6">
-        <v>120.47515200000001</v>
+        <v>117.11951999999999</v>
       </c>
       <c r="H7" s="6">
-        <v>1065.9195359999999</v>
+        <v>1053.2823840000001</v>
       </c>
       <c r="I7" s="6">
-        <v>1089.208944</v>
+        <v>1099.3836960000001</v>
       </c>
       <c r="J7" s="6">
-        <v>65.1708</v>
+        <v>56.244383999999997</v>
       </c>
       <c r="K7" s="6">
-        <v>337.56652800000001</v>
+        <v>336.06864000000002</v>
       </c>
       <c r="L7" s="6">
-        <v>5.6430720000000001</v>
+        <v>12.778560000000001</v>
       </c>
       <c r="M7" s="6">
-        <v>6.9261119999999998</v>
+        <v>2.4566400000000002</v>
       </c>
       <c r="N7" s="6">
-        <v>0</v>
+        <v>2.9087999999999999E-2</v>
       </c>
       <c r="O7" s="6">
-        <v>0.69177600000000006</v>
+        <v>0.68284800000000001</v>
       </c>
       <c r="P7" s="6">
-        <v>721.04846399999997</v>
+        <v>703.99267199999997</v>
       </c>
       <c r="Q7" s="6">
-        <v>1005.7701599999999</v>
+        <v>999.17035199999998</v>
       </c>
       <c r="R7" s="6">
-        <v>304.50974400000001</v>
+        <v>297.726336</v>
       </c>
       <c r="S7" s="6">
-        <v>139.13985600000001</v>
+        <v>165.06503999999998</v>
       </c>
       <c r="T7" s="6">
-        <v>59.86656</v>
+        <v>61.998480000000008</v>
       </c>
       <c r="U7" s="6">
-        <v>21.827664000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+        <v>35.557631999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="6">
-        <v>4.0201919999999998</v>
+        <v>17.642592</v>
       </c>
       <c r="C8" s="6">
-        <v>4.8178080000000003</v>
+        <v>13.057775999999999</v>
       </c>
       <c r="D8" s="6">
-        <v>0</v>
+        <v>0.79358400000000007</v>
       </c>
       <c r="E8" s="6">
-        <v>21.073248</v>
+        <v>19.600848000000003</v>
       </c>
       <c r="F8" s="6">
-        <v>346.80974399999997</v>
+        <v>324.52977599999997</v>
       </c>
       <c r="G8" s="6">
-        <v>29.738159999999997</v>
+        <v>28.668096000000002</v>
       </c>
       <c r="H8" s="6">
-        <v>1034.1293759999999</v>
+        <v>1022.174352</v>
       </c>
       <c r="I8" s="6">
-        <v>1015.5777119999999</v>
+        <v>1013.659632</v>
       </c>
       <c r="J8" s="6">
-        <v>227.52374399999999</v>
+        <v>219.136608</v>
       </c>
       <c r="K8" s="6">
-        <v>47.562480000000001</v>
+        <v>42.170687999999998</v>
       </c>
       <c r="L8" s="6">
-        <v>0</v>
+        <v>7.536816</v>
       </c>
       <c r="M8" s="6">
         <v>0</v>
@@ -3796,26 +3797,47 @@
         <v>0</v>
       </c>
       <c r="O8" s="6">
-        <v>1.794816</v>
+        <v>1.7912159999999999</v>
       </c>
       <c r="P8" s="6">
-        <v>266.49</v>
+        <v>252.63792000000001</v>
       </c>
       <c r="Q8" s="6">
-        <v>430.38864000000001</v>
+        <v>427.13654400000001</v>
       </c>
       <c r="R8" s="6">
-        <v>229.43303999999998</v>
+        <v>223.813008</v>
       </c>
       <c r="S8" s="6">
-        <v>146.10081599999998</v>
+        <v>170.479152</v>
       </c>
       <c r="T8" s="6">
-        <v>53.334143999999995</v>
+        <v>57.435552000000001</v>
       </c>
       <c r="U8" s="6">
-        <v>14.852735999999998</v>
-      </c>
+        <v>31.368384000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>